<commit_message>
figures and meta analysis
</commit_message>
<xml_diff>
--- a/ma_data.xlsx
+++ b/ma_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kathleenowen/Desktop/MSc EEB/WD/metaanalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304BDAC5-0006-DB4A-A85C-AA7C30A4F4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F4EEBF-F146-2E4D-B417-EB973B3B54E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1700" yWindow="1220" windowWidth="27640" windowHeight="16360" xr2:uid="{7CF521C3-AE61-1B4F-B9C7-AD29A3976BC6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="84">
   <si>
     <t>nunavut_archipelago</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
@@ -294,7 +297,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,6 +329,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -347,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -366,6 +377,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,15 +712,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCA7B65B-70AF-2742-B734-C8EB0812CEEB}">
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42:G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -727,8 +739,11 @@
       <c r="F1" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -748,7 +763,7 @@
         <v>43.220300000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -768,7 +783,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -788,7 +803,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
@@ -808,7 +823,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -828,7 +843,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>10</v>
       </c>
@@ -848,7 +863,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
@@ -868,7 +883,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -888,7 +903,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -908,7 +923,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
@@ -928,7 +943,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
@@ -948,7 +963,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
@@ -968,7 +983,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -988,7 +1003,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +1023,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
@@ -1348,7 +1363,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>25</v>
       </c>
@@ -1368,7 +1383,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1403,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>27</v>
       </c>
@@ -1408,7 +1423,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
         <v>27</v>
       </c>
@@ -1428,7 +1443,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>28</v>
       </c>
@@ -1448,7 +1463,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>28</v>
       </c>
@@ -1468,7 +1483,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>29</v>
       </c>
@@ -1488,7 +1503,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>29</v>
       </c>
@@ -1508,7 +1523,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>30</v>
       </c>
@@ -1528,7 +1543,7 @@
         <v>65.421499999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>30</v>
       </c>
@@ -1548,7 +1563,7 @@
         <v>79.833299999999994</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>31</v>
       </c>
@@ -1567,8 +1582,9 @@
       <c r="F43" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>32</v>
       </c>
@@ -1587,8 +1603,9 @@
       <c r="F44" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>33</v>
       </c>
@@ -1607,8 +1624,9 @@
       <c r="F45" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>34</v>
       </c>
@@ -1627,8 +1645,9 @@
       <c r="F46" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
@@ -1647,8 +1666,9 @@
       <c r="F47" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>35</v>
       </c>
@@ -1667,8 +1687,9 @@
       <c r="F48" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="8"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>36</v>
       </c>
@@ -1687,8 +1708,9 @@
       <c r="F49" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="8"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>37</v>
       </c>
@@ -1707,8 +1729,9 @@
       <c r="F50" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>38</v>
       </c>
@@ -1727,8 +1750,9 @@
       <c r="F51" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>39</v>
       </c>
@@ -1747,8 +1771,9 @@
       <c r="F52" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>40</v>
       </c>
@@ -1767,8 +1792,9 @@
       <c r="F53" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
@@ -1787,8 +1813,9 @@
       <c r="F54" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>42</v>
       </c>
@@ -1807,8 +1834,9 @@
       <c r="F55" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>43</v>
       </c>
@@ -1827,8 +1855,9 @@
       <c r="F56" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="8"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>44</v>
       </c>
@@ -1847,8 +1876,9 @@
       <c r="F57" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>45</v>
       </c>
@@ -1867,8 +1897,9 @@
       <c r="F58" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>46</v>
       </c>
@@ -1887,8 +1918,9 @@
       <c r="F59" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" s="8"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>47</v>
       </c>
@@ -1907,8 +1939,9 @@
       <c r="F60" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" s="8"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>48</v>
       </c>
@@ -1927,8 +1960,9 @@
       <c r="F61" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" s="8"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>49</v>
       </c>
@@ -1947,8 +1981,9 @@
       <c r="F62" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" s="8"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>50</v>
       </c>
@@ -1967,8 +2002,9 @@
       <c r="F63" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>51</v>
       </c>
@@ -1987,8 +2023,9 @@
       <c r="F64" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" s="8"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>52</v>
       </c>
@@ -2007,8 +2044,9 @@
       <c r="F65" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65" s="8"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>53</v>
       </c>
@@ -2027,8 +2065,9 @@
       <c r="F66" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" s="8"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>54</v>
       </c>
@@ -2047,8 +2086,9 @@
       <c r="F67" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" s="8"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>55</v>
       </c>
@@ -2067,8 +2107,9 @@
       <c r="F68" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" s="8"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>56</v>
       </c>
@@ -2087,8 +2128,9 @@
       <c r="F69" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" s="8"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>57</v>
       </c>
@@ -2107,8 +2149,9 @@
       <c r="F70" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G70" s="8"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>58</v>
       </c>
@@ -2127,8 +2170,9 @@
       <c r="F71" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" s="8"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>59</v>
       </c>
@@ -2147,8 +2191,9 @@
       <c r="F72" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" s="8"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>60</v>
       </c>
@@ -2167,8 +2212,9 @@
       <c r="F73" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G73" s="8"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>61</v>
       </c>
@@ -2187,8 +2233,9 @@
       <c r="F74" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G74" s="8"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>62</v>
       </c>
@@ -2207,8 +2254,9 @@
       <c r="F75" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G75" s="8"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>63</v>
       </c>
@@ -2227,8 +2275,9 @@
       <c r="F76" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76" s="8"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>64</v>
       </c>
@@ -2247,8 +2296,9 @@
       <c r="F77" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77" s="8"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>65</v>
       </c>
@@ -2267,8 +2317,9 @@
       <c r="F78" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G78" s="8"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
         <v>66</v>
       </c>
@@ -2287,8 +2338,9 @@
       <c r="F79" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G79" s="8"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>67</v>
       </c>
@@ -2307,8 +2359,9 @@
       <c r="F80" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" s="8"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>68</v>
       </c>
@@ -2327,8 +2380,9 @@
       <c r="F81" s="2">
         <v>38.958300000000001</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G81" s="8"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>69</v>
       </c>
@@ -2348,7 +2402,7 @@
         <v>74.466999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>70</v>
       </c>
@@ -2368,7 +2422,7 @@
         <v>74.466999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>71</v>
       </c>
@@ -2388,7 +2442,7 @@
         <v>74.466999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
         <v>72</v>
       </c>
@@ -2408,7 +2462,7 @@
         <v>74.466999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
         <v>73</v>
       </c>
@@ -2428,7 +2482,7 @@
         <v>74.466999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>74</v>
       </c>

</xml_diff>